<commit_message>
penambahan data yang di analisa penambahan materi untuk bab III
</commit_message>
<xml_diff>
--- a/PROSKRIP/Analisa_LK_UNVR_2014_2018.xlsx
+++ b/PROSKRIP/Analisa_LK_UNVR_2014_2018.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ANALISIS" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="85">
   <si>
     <t>Kas dan setara kas</t>
   </si>
@@ -300,6 +300,12 @@
   <si>
     <t xml:space="preserve">Harga penutupan </t>
   </si>
+  <si>
+    <t>Ekuitas</t>
+  </si>
+  <si>
+    <t>Liabilitas &amp; Ekuitas</t>
+  </si>
 </sst>
 </file>
 
@@ -308,8 +314,8 @@
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="170" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;????_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;????_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -414,104 +420,89 @@
   </cellStyleXfs>
   <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -524,13 +515,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -816,370 +822,464 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="70.7109375" style="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="37" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="13.28515625" style="37" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.7109375" style="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="13.28515625" style="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="34" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="2:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="41"/>
-      <c r="C2" s="40" t="s">
+      <c r="C1" s="42" t="str">
+        <f>IF(C8-C15=0,"","X")</f>
+        <v/>
+      </c>
+      <c r="D1" s="42" t="str">
+        <f>IF(D8-D15=0,"","X")</f>
+        <v/>
+      </c>
+      <c r="E1" s="42" t="str">
+        <f>IF(E8-E15=0,"","X")</f>
+        <v/>
+      </c>
+      <c r="F1" s="42" t="str">
+        <f>IF(F8-F15=0,"","X")</f>
+        <v/>
+      </c>
+      <c r="G1" s="42" t="str">
+        <f>IF(G8-G15=0,"","X")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="2" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="36"/>
+      <c r="C2" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="35" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="46" t="s">
+    <row r="3" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="47">
+      <c r="C3" s="42">
         <f>BALANCE_SHEET!E19</f>
         <v>6337170</v>
       </c>
-      <c r="D3" s="47">
+      <c r="D3" s="42">
         <f>BALANCE_SHEET!F19</f>
         <v>6623114</v>
       </c>
-      <c r="E3" s="47">
+      <c r="E3" s="42">
         <f>BALANCE_SHEET!G19</f>
         <v>6588109</v>
       </c>
-      <c r="F3" s="47">
+      <c r="F3" s="42">
         <f>BALANCE_SHEET!H19</f>
         <v>7941635</v>
       </c>
-      <c r="G3" s="47">
+      <c r="G3" s="42">
         <f>BALANCE_SHEET!I19</f>
         <v>8325029</v>
       </c>
     </row>
-    <row r="4" spans="2:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="46" t="s">
+    <row r="4" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="47">
+      <c r="C4" s="42">
         <f>BALANCE_SHEET!E22</f>
         <v>7348025</v>
       </c>
-      <c r="D4" s="47">
+      <c r="D4" s="42">
         <f>BALANCE_SHEET!F22</f>
         <v>8320917</v>
       </c>
-      <c r="E4" s="47">
+      <c r="E4" s="42">
         <f>BALANCE_SHEET!G22</f>
         <v>9529476</v>
       </c>
-      <c r="F4" s="47">
+      <c r="F4" s="42">
         <f>BALANCE_SHEET!H22</f>
         <v>10422133</v>
       </c>
-      <c r="G4" s="47">
+      <c r="G4" s="42">
         <f>BALANCE_SHEET!I22</f>
         <v>10627387</v>
       </c>
     </row>
-    <row r="5" spans="2:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="46" t="s">
+    <row r="5" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="47">
+      <c r="C5" s="42">
         <f>BALANCE_SHEET!E23</f>
         <v>61925</v>
       </c>
-      <c r="D5" s="47">
+      <c r="D5" s="42">
         <f>BALANCE_SHEET!F23</f>
         <v>61925</v>
       </c>
-      <c r="E5" s="47">
+      <c r="E5" s="42">
         <f>BALANCE_SHEET!G23</f>
         <v>61925</v>
       </c>
-      <c r="F5" s="47">
+      <c r="F5" s="42">
         <f>BALANCE_SHEET!H23</f>
         <v>61925</v>
       </c>
-      <c r="G5" s="47">
+      <c r="G5" s="42">
         <f>BALANCE_SHEET!I23</f>
         <v>61925</v>
       </c>
     </row>
-    <row r="6" spans="2:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="46" t="s">
+    <row r="6" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="47">
+      <c r="C6" s="42">
         <f>BALANCE_SHEET!E24</f>
         <v>452240</v>
       </c>
-      <c r="D6" s="47">
+      <c r="D6" s="42">
         <f>BALANCE_SHEET!F24</f>
         <v>431021</v>
       </c>
-      <c r="E6" s="47">
+      <c r="E6" s="42">
         <f>BALANCE_SHEET!G24</f>
         <v>409802</v>
       </c>
-      <c r="F6" s="47">
+      <c r="F6" s="42">
         <f>BALANCE_SHEET!H24</f>
         <v>390838</v>
       </c>
-      <c r="G6" s="47">
+      <c r="G6" s="42">
         <f>BALANCE_SHEET!I24</f>
         <v>434205</v>
       </c>
     </row>
-    <row r="7" spans="2:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="46" t="s">
+    <row r="7" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="47">
+      <c r="C7" s="42">
         <f>BALANCE_SHEET!E25</f>
         <v>81310</v>
       </c>
-      <c r="D7" s="47">
+      <c r="D7" s="42">
         <f>BALANCE_SHEET!F25</f>
         <v>292968</v>
       </c>
-      <c r="E7" s="47">
+      <c r="E7" s="42">
         <f>BALANCE_SHEET!G25</f>
         <v>156383</v>
       </c>
-      <c r="F7" s="47">
+      <c r="F7" s="42">
         <f>BALANCE_SHEET!H25</f>
         <v>89882</v>
       </c>
-      <c r="G7" s="47">
+      <c r="G7" s="42">
         <f>BALANCE_SHEET!I25</f>
         <v>74424</v>
       </c>
     </row>
-    <row r="8" spans="2:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="46" t="s">
+    <row r="8" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="C8" s="47">
+      <c r="C8" s="42">
         <f>SUM(C3:C7)</f>
         <v>14280670</v>
       </c>
-      <c r="D8" s="47">
+      <c r="D8" s="42">
         <f t="shared" ref="D8:G8" si="0">SUM(D3:D7)</f>
         <v>15729945</v>
       </c>
-      <c r="E8" s="47">
+      <c r="E8" s="42">
         <f t="shared" si="0"/>
         <v>16745695</v>
       </c>
-      <c r="F8" s="47">
+      <c r="F8" s="42">
         <f t="shared" si="0"/>
         <v>18906413</v>
       </c>
-      <c r="G8" s="47">
+      <c r="G8" s="42">
         <f t="shared" si="0"/>
         <v>19522970</v>
       </c>
     </row>
-    <row r="9" spans="2:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="46"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-    </row>
-    <row r="10" spans="2:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="46" t="s">
+    <row r="9" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="41"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+    </row>
+    <row r="10" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-    </row>
-    <row r="11" spans="2:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="46" t="s">
+      <c r="C10" s="42">
+        <f>BALANCE_SHEET!E43</f>
+        <v>8864832</v>
+      </c>
+      <c r="D10" s="42">
+        <f>BALANCE_SHEET!F43</f>
+        <v>10127542</v>
+      </c>
+      <c r="E10" s="42">
+        <f>BALANCE_SHEET!G43</f>
+        <v>10878074</v>
+      </c>
+      <c r="F10" s="42">
+        <f>BALANCE_SHEET!H43</f>
+        <v>12532304</v>
+      </c>
+      <c r="G10" s="42">
+        <f>BALANCE_SHEET!I43</f>
+        <v>11134786</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
-    </row>
-    <row r="12" spans="2:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="46" t="s">
+      <c r="C11" s="42">
+        <f>BALANCE_SHEET!E48</f>
+        <v>817056</v>
+      </c>
+      <c r="D11" s="42">
+        <f>BALANCE_SHEET!F48</f>
+        <v>775043</v>
+      </c>
+      <c r="E11" s="42">
+        <f>BALANCE_SHEET!G48</f>
+        <v>1163363</v>
+      </c>
+      <c r="F11" s="42">
+        <f>BALANCE_SHEET!H48</f>
+        <v>1200721</v>
+      </c>
+      <c r="G11" s="42">
+        <f>BALANCE_SHEET!I48</f>
+        <v>810051</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="47"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
-    </row>
-    <row r="13" spans="2:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="46"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-    </row>
-    <row r="14" spans="2:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="46"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-    </row>
-    <row r="15" spans="2:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="46"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="47"/>
-    </row>
-    <row r="16" spans="2:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="46"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
-    </row>
-    <row r="17" spans="2:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="46"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-    </row>
-    <row r="18" spans="2:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="46"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
-    </row>
-    <row r="19" spans="2:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="46" t="s">
+      <c r="C12" s="42">
+        <f>C10+C11</f>
+        <v>9681888</v>
+      </c>
+      <c r="D12" s="42">
+        <f>D10+D11</f>
+        <v>10902585</v>
+      </c>
+      <c r="E12" s="42">
+        <f>E10+E11</f>
+        <v>12041437</v>
+      </c>
+      <c r="F12" s="42">
+        <f>F10+F11</f>
+        <v>13733025</v>
+      </c>
+      <c r="G12" s="42">
+        <f>G10+G11</f>
+        <v>11944837</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="41"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+    </row>
+    <row r="14" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="42">
+        <f>BALANCE_SHEET!E57</f>
+        <v>4598782</v>
+      </c>
+      <c r="D14" s="42">
+        <f>BALANCE_SHEET!F57</f>
+        <v>4827360</v>
+      </c>
+      <c r="E14" s="42">
+        <f>BALANCE_SHEET!G57</f>
+        <v>4704258</v>
+      </c>
+      <c r="F14" s="42">
+        <f>BALANCE_SHEET!H57</f>
+        <v>5173388</v>
+      </c>
+      <c r="G14" s="42">
+        <f>BALANCE_SHEET!I57</f>
+        <v>7578133</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="42">
+        <f>C12+C14</f>
+        <v>14280670</v>
+      </c>
+      <c r="D15" s="42">
+        <f t="shared" ref="D15:G15" si="1">D12+D14</f>
+        <v>15729945</v>
+      </c>
+      <c r="E15" s="42">
+        <f t="shared" si="1"/>
+        <v>16745695</v>
+      </c>
+      <c r="F15" s="42">
+        <f t="shared" si="1"/>
+        <v>18906413</v>
+      </c>
+      <c r="G15" s="42">
+        <f t="shared" si="1"/>
+        <v>19522970</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="41"/>
+    </row>
+    <row r="17" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="41"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+    </row>
+    <row r="18" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="41"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+    </row>
+    <row r="19" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47">
+      <c r="C19" s="42"/>
+      <c r="D19" s="42">
         <v>37000</v>
       </c>
-      <c r="E19" s="47">
+      <c r="E19" s="42">
         <v>38800</v>
       </c>
       <c r="F19">
         <v>55900</v>
       </c>
-      <c r="G19" s="47">
+      <c r="G19" s="42">
         <v>45400</v>
       </c>
     </row>
-    <row r="20" spans="2:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="46"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="47"/>
-    </row>
-    <row r="21" spans="2:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="46"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-    </row>
-    <row r="22" spans="2:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="46"/>
-      <c r="C22" s="47"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="47"/>
-    </row>
-    <row r="23" spans="2:7" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="46" t="s">
+    <row r="20" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="41"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+    </row>
+    <row r="21" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="41"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+    </row>
+    <row r="22" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="41"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+    </row>
+    <row r="23" spans="2:7" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="44">
+      <c r="C23" s="39">
         <f>INCOME_STATEMENT!D6</f>
         <v>34511534</v>
       </c>
-      <c r="D23" s="44">
+      <c r="D23" s="39">
         <f>INCOME_STATEMENT!E6</f>
         <v>36484030</v>
       </c>
-      <c r="E23" s="44">
+      <c r="E23" s="39">
         <f>INCOME_STATEMENT!F6</f>
         <v>40053732</v>
       </c>
-      <c r="F23" s="44">
+      <c r="F23" s="39">
         <f>INCOME_STATEMENT!G6</f>
         <v>41204510</v>
       </c>
-      <c r="G23" s="44">
+      <c r="G23" s="39">
         <f>INCOME_STATEMENT!H6</f>
         <v>41802073</v>
       </c>
     </row>
-    <row r="24" spans="2:7" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="46" t="s">
+    <row r="24" spans="2:7" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="C24" s="44">
+      <c r="C24" s="39">
         <f>INCOME_STATEMENT!D17</f>
         <v>5738523</v>
       </c>
-      <c r="D24" s="44">
+      <c r="D24" s="39">
         <f>INCOME_STATEMENT!E17</f>
         <v>5851805</v>
       </c>
-      <c r="E24" s="44">
+      <c r="E24" s="39">
         <f>INCOME_STATEMENT!F17</f>
         <v>6390672</v>
       </c>
-      <c r="F24" s="44">
+      <c r="F24" s="39">
         <f>INCOME_STATEMENT!G17</f>
         <v>7004562</v>
       </c>
-      <c r="G24" s="44">
+      <c r="G24" s="39">
         <f>INCOME_STATEMENT!H17</f>
         <v>9109445</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="46" t="s">
+      <c r="B25" s="41" t="s">
         <v>76</v>
       </c>
       <c r="C25" s="2">
@@ -1204,84 +1304,84 @@
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="42"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="43" t="s">
+      <c r="B27" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="37">
+      <c r="C27" s="32">
         <f>INCOME_STATEMENT!D17/BALANCE_SHEET!E27</f>
         <v>0.40183849917405834</v>
       </c>
-      <c r="D27" s="37">
+      <c r="D27" s="32">
         <f>INCOME_STATEMENT!E17/BALANCE_SHEET!F27</f>
         <v>0.37201687609206519</v>
       </c>
-      <c r="E27" s="37">
+      <c r="E27" s="32">
         <f>INCOME_STATEMENT!F17/BALANCE_SHEET!G27</f>
         <v>0.38163074151296794</v>
       </c>
-      <c r="F27" s="37">
+      <c r="F27" s="32">
         <f>INCOME_STATEMENT!G17/BALANCE_SHEET!H27</f>
         <v>0.37048603561130289</v>
       </c>
-      <c r="G27" s="37">
+      <c r="G27" s="32">
         <f>INCOME_STATEMENT!H17/BALANCE_SHEET!I27</f>
         <v>0.46660139312819721</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="43" t="s">
+      <c r="B28" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="C28" s="37">
+      <c r="C28" s="32">
         <f>BALANCE_SHEET!E49/BALANCE_SHEET!E57</f>
         <v>2.1053157118558783</v>
       </c>
-      <c r="D28" s="37">
+      <c r="D28" s="32">
         <f>BALANCE_SHEET!F49/BALANCE_SHEET!F57</f>
         <v>2.2584984339266181</v>
       </c>
-      <c r="E28" s="37">
+      <c r="E28" s="32">
         <f>BALANCE_SHEET!G49/BALANCE_SHEET!G57</f>
         <v>2.5596889031171335</v>
       </c>
-      <c r="F28" s="37">
+      <c r="F28" s="32">
         <f>BALANCE_SHEET!H49/BALANCE_SHEET!H57</f>
         <v>2.6545515240689466</v>
       </c>
-      <c r="G28" s="37">
+      <c r="G28" s="32">
         <f>BALANCE_SHEET!I49/BALANCE_SHEET!I57</f>
         <v>1.576224249429246</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="43" t="s">
+      <c r="B29" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="C29" s="37">
+      <c r="C29" s="32">
         <f>INCOME_STATEMENT!D17/INCOME_STATEMENT!D6</f>
         <v>0.16627840999475713</v>
       </c>
-      <c r="D29" s="37">
+      <c r="D29" s="32">
         <f>INCOME_STATEMENT!E17/INCOME_STATEMENT!E6</f>
         <v>0.16039360235149461</v>
       </c>
-      <c r="E29" s="37">
+      <c r="E29" s="32">
         <f>INCOME_STATEMENT!F17/INCOME_STATEMENT!F6</f>
         <v>0.15955247316280041</v>
       </c>
-      <c r="F29" s="37">
+      <c r="F29" s="32">
         <f>INCOME_STATEMENT!G17/INCOME_STATEMENT!G6</f>
         <v>0.16999503209721459</v>
       </c>
-      <c r="G29" s="37">
+      <c r="G29" s="32">
         <f>INCOME_STATEMENT!H17/INCOME_STATEMENT!H6</f>
         <v>0.21791849892229029</v>
       </c>
@@ -1296,99 +1396,99 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I59"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="8"/>
     <col min="2" max="2" width="3.28515625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="3.28515625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="29.5703125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="3.28515625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="29.5703125" style="10" customWidth="1"/>
     <col min="5" max="9" width="12.140625" style="8" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="20" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="20" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="29" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="2:9" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="35"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="20" t="str">
+    <row r="4" spans="2:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="30"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="16" t="str">
         <f>IF(E27-E58=0,"BALANCED","unbalanced")</f>
         <v>BALANCED</v>
       </c>
-      <c r="F4" s="20" t="str">
+      <c r="F4" s="16" t="str">
         <f>IF(F27-F58=0,"BALANCED","unbalanced")</f>
         <v>BALANCED</v>
       </c>
-      <c r="G4" s="20" t="str">
+      <c r="G4" s="16" t="str">
         <f>IF(G27-G58=0,"BALANCED","unbalanced")</f>
         <v>BALANCED</v>
       </c>
-      <c r="H4" s="20" t="str">
+      <c r="H4" s="16" t="str">
         <f>IF(H27-H58=0,"BALANCED","unbalanced")</f>
         <v>BALANCED</v>
       </c>
-      <c r="I4" s="20" t="str">
+      <c r="I4" s="16" t="str">
         <f>IF(I27-I58=0,"BALANCED","unbalanced")</f>
         <v>BALANCED</v>
       </c>
     </row>
     <row r="5" spans="2:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="17"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="19" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
     </row>
     <row r="7" spans="2:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="10"/>
+      <c r="D8" s="46"/>
       <c r="E8" s="8">
         <v>859127</v>
       </c>
@@ -1406,13 +1506,13 @@
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="10"/>
+      <c r="D9" s="46"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="10" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="8">
@@ -1432,7 +1532,7 @@
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E11" s="8">
@@ -1452,13 +1552,13 @@
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="10"/>
+      <c r="D12" s="46"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="10" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="8">
@@ -1478,7 +1578,7 @@
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E14" s="8">
@@ -1498,10 +1598,10 @@
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="10"/>
+      <c r="D15" s="46"/>
       <c r="E15" s="8">
         <v>2325989</v>
       </c>
@@ -1519,10 +1619,10 @@
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="10"/>
+      <c r="D16" s="46"/>
       <c r="E16" s="8">
         <f>14179+85615</f>
         <v>99794</v>
@@ -1535,10 +1635,10 @@
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="10"/>
+      <c r="D17" s="46"/>
       <c r="E17" s="8">
         <v>0</v>
       </c>
@@ -1556,10 +1656,10 @@
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="10"/>
+      <c r="D18" s="46"/>
       <c r="E18" s="8">
         <v>0</v>
       </c>
@@ -1580,8 +1680,8 @@
       <c r="B19" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
       <c r="E19" s="6">
         <f>SUM(E8:E18)</f>
         <v>6337170</v>
@@ -1607,14 +1707,14 @@
       <c r="B21" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="10"/>
+      <c r="D22" s="46"/>
       <c r="E22" s="8">
         <v>7348025</v>
       </c>
@@ -1632,10 +1732,10 @@
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C23" s="48" t="s">
+      <c r="C23" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="48"/>
+      <c r="D23" s="47"/>
       <c r="E23" s="8">
         <v>61925</v>
       </c>
@@ -1653,10 +1753,10 @@
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="10"/>
+      <c r="D24" s="46"/>
       <c r="E24" s="8">
         <v>452240</v>
       </c>
@@ -1674,10 +1774,10 @@
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="10"/>
+      <c r="D25" s="46"/>
       <c r="E25" s="8">
         <v>81310</v>
       </c>
@@ -1698,8 +1798,8 @@
       <c r="B26" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
       <c r="E26" s="6">
         <f>SUM(E22:E25)</f>
         <v>7943500</v>
@@ -1721,29 +1821,29 @@
         <v>11197941</v>
       </c>
     </row>
-    <row r="27" spans="2:9" s="14" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="16" t="s">
+    <row r="27" spans="2:9" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="13">
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="11">
         <f>E19+E26</f>
         <v>14280670</v>
       </c>
-      <c r="F27" s="13">
+      <c r="F27" s="11">
         <f t="shared" ref="F27:I27" si="1">F19+F26</f>
         <v>15729945</v>
       </c>
-      <c r="G27" s="13">
+      <c r="G27" s="11">
         <f t="shared" si="1"/>
         <v>16745695</v>
       </c>
-      <c r="H27" s="13">
+      <c r="H27" s="11">
         <f t="shared" si="1"/>
         <v>18906413</v>
       </c>
-      <c r="I27" s="13">
+      <c r="I27" s="11">
         <f t="shared" si="1"/>
         <v>19522970</v>
       </c>
@@ -1760,10 +1860,10 @@
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="10"/>
+      <c r="D31" s="46"/>
       <c r="E31" s="8">
         <v>1250000</v>
       </c>
@@ -1781,13 +1881,13 @@
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="D32" s="10"/>
+      <c r="D32" s="46"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D33" s="12" t="s">
+      <c r="D33" s="10" t="s">
         <v>2</v>
       </c>
       <c r="E33" s="8">
@@ -1807,7 +1907,7 @@
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E34" s="8">
@@ -1827,13 +1927,13 @@
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="D35" s="10"/>
+      <c r="D35" s="46"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D36" s="12" t="s">
+      <c r="D36" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E36" s="8">
@@ -1853,7 +1953,7 @@
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D37" s="12" t="s">
+      <c r="D37" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E37" s="8">
@@ -1873,10 +1973,10 @@
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C38" s="10" t="s">
+      <c r="C38" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="D38" s="10"/>
+      <c r="D38" s="46"/>
       <c r="E38" s="8">
         <v>1141375</v>
       </c>
@@ -1894,13 +1994,13 @@
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C39" s="10" t="s">
+      <c r="C39" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="D39" s="10"/>
+      <c r="D39" s="46"/>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D40" s="12" t="s">
+      <c r="D40" s="10" t="s">
         <v>2</v>
       </c>
       <c r="E40" s="8">
@@ -1920,7 +2020,7 @@
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D41" s="12" t="s">
+      <c r="D41" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E41" s="8">
@@ -1940,10 +2040,10 @@
       </c>
     </row>
     <row r="42" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C42" s="10" t="s">
+      <c r="C42" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="D42" s="10"/>
+      <c r="D42" s="46"/>
       <c r="E42" s="8">
         <v>39034</v>
       </c>
@@ -1964,8 +2064,8 @@
       <c r="B43" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
       <c r="E43" s="6">
         <f>SUM(E31:E42)</f>
         <v>8864832</v>
@@ -1993,10 +2093,10 @@
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C46" s="10" t="s">
+      <c r="C46" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="D46" s="10"/>
+      <c r="D46" s="46"/>
       <c r="E46" s="8">
         <v>246093</v>
       </c>
@@ -2014,10 +2114,10 @@
       </c>
     </row>
     <row r="47" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C47" s="10" t="s">
+      <c r="C47" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="D47" s="10"/>
+      <c r="D47" s="46"/>
       <c r="E47" s="8">
         <v>570963</v>
       </c>
@@ -2038,8 +2138,8 @@
       <c r="B48" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
       <c r="E48" s="6">
         <f>SUM(E46:E47)</f>
         <v>817056</v>
@@ -2062,28 +2162,28 @@
       </c>
     </row>
     <row r="49" spans="2:9" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="16" t="s">
+      <c r="B49" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="C49" s="16"/>
-      <c r="D49" s="16"/>
-      <c r="E49" s="13">
+      <c r="C49" s="45"/>
+      <c r="D49" s="45"/>
+      <c r="E49" s="11">
         <f>E43+E48</f>
         <v>9681888</v>
       </c>
-      <c r="F49" s="13">
+      <c r="F49" s="11">
         <f>F43+F48</f>
         <v>10902585</v>
       </c>
-      <c r="G49" s="13">
+      <c r="G49" s="11">
         <f t="shared" ref="G49:I49" si="3">G43+G48</f>
         <v>12041437</v>
       </c>
-      <c r="H49" s="13">
+      <c r="H49" s="11">
         <f t="shared" si="3"/>
         <v>13733025</v>
       </c>
-      <c r="I49" s="13">
+      <c r="I49" s="11">
         <f t="shared" si="3"/>
         <v>11944837</v>
       </c>
@@ -2093,17 +2193,17 @@
       <c r="B51" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C52" s="10" t="s">
+      <c r="C52" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="D52" s="10"/>
+      <c r="D52" s="46"/>
     </row>
     <row r="53" spans="2:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D53" s="49" t="s">
+      <c r="D53" s="43" t="s">
         <v>40</v>
       </c>
       <c r="E53" s="5">
@@ -2123,10 +2223,10 @@
       </c>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C54" s="10" t="s">
+      <c r="C54" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="D54" s="10"/>
+      <c r="D54" s="46"/>
       <c r="E54" s="8">
         <v>96000</v>
       </c>
@@ -2144,10 +2244,10 @@
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C55" s="10" t="s">
+      <c r="C55" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="D55" s="10"/>
+      <c r="D55" s="46"/>
       <c r="E55" s="8">
         <v>15260</v>
       </c>
@@ -2165,10 +2265,10 @@
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C56" s="10" t="s">
+      <c r="C56" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="D56" s="10"/>
+      <c r="D56" s="46"/>
       <c r="E56" s="8">
         <v>4411222</v>
       </c>
@@ -2186,55 +2286,55 @@
       </c>
     </row>
     <row r="57" spans="2:9" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="16" t="s">
+      <c r="B57" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="C57" s="16"/>
-      <c r="D57" s="16"/>
-      <c r="E57" s="13">
+      <c r="C57" s="45"/>
+      <c r="D57" s="45"/>
+      <c r="E57" s="11">
         <f>SUM(E52:E56)</f>
         <v>4598782</v>
       </c>
-      <c r="F57" s="13">
-        <f t="shared" ref="F57:I57" si="4">SUM(F52:F56)</f>
+      <c r="F57" s="11">
+        <f t="shared" ref="F57:G57" si="4">SUM(F52:F56)</f>
         <v>4827360</v>
       </c>
-      <c r="G57" s="13">
+      <c r="G57" s="11">
         <f t="shared" si="4"/>
         <v>4704258</v>
       </c>
-      <c r="H57" s="13">
+      <c r="H57" s="11">
         <f>SUM(H53:H56)</f>
         <v>5173388</v>
       </c>
-      <c r="I57" s="13">
+      <c r="I57" s="11">
         <f>SUM(I53:I56)</f>
         <v>7578133</v>
       </c>
     </row>
     <row r="58" spans="2:9" s="6" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="16" t="s">
+      <c r="B58" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="C58" s="16"/>
-      <c r="D58" s="16"/>
-      <c r="E58" s="13">
+      <c r="C58" s="45"/>
+      <c r="D58" s="45"/>
+      <c r="E58" s="11">
         <f>E49+E57</f>
         <v>14280670</v>
       </c>
-      <c r="F58" s="13">
+      <c r="F58" s="11">
         <f>F49+F57</f>
         <v>15729945</v>
       </c>
-      <c r="G58" s="13">
+      <c r="G58" s="11">
         <f>G49+G57</f>
         <v>16745695</v>
       </c>
-      <c r="H58" s="13">
+      <c r="H58" s="11">
         <f>H49+H57</f>
         <v>18906413</v>
       </c>
-      <c r="I58" s="13">
+      <c r="I58" s="11">
         <f>I49+I57</f>
         <v>19522970</v>
       </c>
@@ -2242,6 +2342,18 @@
     <row r="59" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C23:D23"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B27:D27"/>
     <mergeCell ref="B49:D49"/>
@@ -2258,18 +2370,6 @@
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C23:D23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2287,63 +2387,63 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="3.7109375" style="23" customWidth="1"/>
-    <col min="3" max="3" width="41.5703125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="3.7109375" style="19" customWidth="1"/>
+    <col min="3" max="3" width="41.5703125" style="10" customWidth="1"/>
     <col min="4" max="8" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="11"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="9"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="32"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
     </row>
     <row r="5" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="26"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="28" t="s">
+      <c r="B5" s="22"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="F5" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="9"/>
+      <c r="C6" s="48"/>
       <c r="D6" s="1">
         <v>34511534</v>
       </c>
@@ -2361,10 +2461,10 @@
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="9"/>
+      <c r="C7" s="48"/>
       <c r="D7" s="1">
         <v>-17412413</v>
       </c>
@@ -2382,8 +2482,8 @@
       </c>
     </row>
     <row r="8" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="24"/>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="20"/>
+      <c r="C8" s="9" t="s">
         <v>49</v>
       </c>
       <c r="D8" s="3">
@@ -2408,10 +2508,10 @@
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="9"/>
+      <c r="C9" s="48"/>
       <c r="D9" s="1">
         <v>-6613992</v>
       </c>
@@ -2429,10 +2529,10 @@
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="9"/>
+      <c r="C10" s="48"/>
       <c r="D10" s="1">
         <v>-2705822</v>
       </c>
@@ -2450,10 +2550,10 @@
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="9"/>
+      <c r="C11" s="48"/>
       <c r="D11" s="1">
         <v>-16979</v>
       </c>
@@ -2471,8 +2571,8 @@
       </c>
     </row>
     <row r="12" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="24"/>
-      <c r="C12" s="11" t="s">
+      <c r="B12" s="20"/>
+      <c r="C12" s="9" t="s">
         <v>52</v>
       </c>
       <c r="D12" s="3">
@@ -2497,10 +2597,10 @@
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="9"/>
+      <c r="C13" s="48"/>
       <c r="D13" s="1">
         <v>10458</v>
       </c>
@@ -2518,10 +2618,10 @@
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="9"/>
+      <c r="C14" s="48"/>
       <c r="D14" s="1">
         <v>-96064</v>
       </c>
@@ -2539,8 +2639,8 @@
       </c>
     </row>
     <row r="15" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="24"/>
-      <c r="C15" s="11" t="s">
+      <c r="B15" s="20"/>
+      <c r="C15" s="9" t="s">
         <v>55</v>
       </c>
       <c r="D15" s="3">
@@ -2565,10 +2665,10 @@
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="9"/>
+      <c r="C16" s="48"/>
       <c r="D16" s="1">
         <v>-1938199</v>
       </c>
@@ -2586,8 +2686,8 @@
       </c>
     </row>
     <row r="17" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="24"/>
-      <c r="C17" s="11" t="s">
+      <c r="B17" s="20"/>
+      <c r="C17" s="9" t="s">
         <v>57</v>
       </c>
       <c r="D17" s="3">
@@ -2612,19 +2712,19 @@
       </c>
     </row>
     <row r="18" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="15"/>
+      <c r="C18" s="44"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="9"/>
+      <c r="C19" s="48"/>
     </row>
     <row r="20" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="10" t="s">
         <v>61</v>
       </c>
       <c r="D20" s="1">
@@ -2644,7 +2744,7 @@
       </c>
     </row>
     <row r="21" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="10" t="s">
         <v>62</v>
       </c>
       <c r="D21" s="1">
@@ -2664,10 +2764,10 @@
       </c>
     </row>
     <row r="22" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="15"/>
+      <c r="C22" s="44"/>
       <c r="D22" s="3">
         <f>D20+D21</f>
         <v>0</v>
@@ -2690,10 +2790,10 @@
       </c>
     </row>
     <row r="23" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="15"/>
+      <c r="C23" s="44"/>
       <c r="D23" s="3">
         <f>D17+D22</f>
         <v>5738523</v>
@@ -2715,35 +2815,35 @@
         <v>9386195</v>
       </c>
     </row>
-    <row r="24" spans="2:8" s="25" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="29" t="s">
+    <row r="24" spans="2:8" s="21" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="29"/>
-      <c r="D24" s="25">
+      <c r="C24" s="49"/>
+      <c r="D24" s="21">
         <v>0</v>
       </c>
-      <c r="E24" s="25">
+      <c r="E24" s="21">
         <v>0</v>
       </c>
-      <c r="F24" s="25">
+      <c r="F24" s="21">
         <v>0</v>
       </c>
-      <c r="G24" s="25">
+      <c r="G24" s="21">
         <v>10149844</v>
       </c>
-      <c r="H24" s="25">
+      <c r="H24" s="21">
         <v>13055881</v>
       </c>
     </row>
     <row r="25" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C25" s="15"/>
+      <c r="C25" s="44"/>
     </row>
     <row r="26" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="10" t="s">
         <v>66</v>
       </c>
       <c r="D26" s="1">
@@ -2764,12 +2864,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B24:C24"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B9:C9"/>
@@ -2778,6 +2872,12 @@
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B24:C24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>